<commit_message>
Render crowded scatterplot solutions on poster panel maps
</commit_message>
<xml_diff>
--- a/A_Inputs/poster_dims.xlsx
+++ b/A_Inputs/poster_dims.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/crowded_scatterplot/A_Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C274249-DCF7-7749-9E8E-F9F28B08DF18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD51B123-AA6C-1F4F-9CC3-FE635D649DA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6220" windowWidth="11800" windowHeight="14040" xr2:uid="{2042E96D-9F05-8D48-B2D5-FC97503682BC}"/>
+    <workbookView xWindow="11120" yWindow="940" windowWidth="16840" windowHeight="20340" xr2:uid="{2042E96D-9F05-8D48-B2D5-FC97503682BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -177,6 +177,13 @@
     <font>
       <sz val="12"/>
       <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -202,12 +209,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,7 +533,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,7 +669,7 @@
         <v>37</v>
       </c>
       <c r="I4">
-        <v>1.6</v>
+        <v>1.6015600000000001</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -811,12 +819,12 @@
         <f>C11+B11</f>
         <v>11.5</v>
       </c>
-      <c r="E11">
-        <v>0.5</v>
+      <c r="E11" s="3">
+        <v>0.7</v>
       </c>
       <c r="F11">
         <f>G12</f>
-        <v>23</v>
+        <v>22.8</v>
       </c>
       <c r="G11">
         <f t="shared" ref="G11:G16" si="2">F11+E11</f>
@@ -842,15 +850,15 @@
       </c>
       <c r="E12">
         <f>B12/$I$4</f>
-        <v>6.875</v>
+        <v>6.8683034041809234</v>
       </c>
       <c r="F12">
         <f>G13</f>
-        <v>16.125</v>
+        <v>15.931696595819076</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>22.8</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -871,7 +879,7 @@
       </c>
       <c r="E13">
         <f>$I$3-E12-E11</f>
-        <v>3.625</v>
+        <v>3.4316965958190764</v>
       </c>
       <c r="F13">
         <f>$G$3</f>
@@ -879,7 +887,7 @@
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
-        <v>16.125</v>
+        <v>15.931696595819076</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -899,11 +907,12 @@
         <v>11.5</v>
       </c>
       <c r="E14">
-        <v>0.5</v>
+        <f>E11</f>
+        <v>0.7</v>
       </c>
       <c r="F14">
         <f>G15</f>
-        <v>11</v>
+        <v>10.8</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
@@ -928,15 +937,15 @@
       </c>
       <c r="E15">
         <f>B15/$I$4</f>
-        <v>6.875</v>
+        <v>6.8683034041809234</v>
       </c>
       <c r="F15">
         <f>G16</f>
-        <v>4.125</v>
+        <v>3.9316965958190764</v>
       </c>
       <c r="G15">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -957,7 +966,7 @@
       </c>
       <c r="E16">
         <f>$I$3-E15-E14</f>
-        <v>3.625</v>
+        <v>3.4316965958190764</v>
       </c>
       <c r="F16">
         <f>$G$4</f>
@@ -965,7 +974,7 @@
       </c>
       <c r="G16">
         <f t="shared" si="2"/>
-        <v>4.125</v>
+        <v>3.9316965958190764</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -990,11 +999,12 @@
         <v>23.5</v>
       </c>
       <c r="E18">
-        <v>0.5</v>
+        <f>E11</f>
+        <v>0.7</v>
       </c>
       <c r="F18">
         <f>G19</f>
-        <v>23</v>
+        <v>22.8</v>
       </c>
       <c r="G18">
         <f t="shared" ref="G18:G23" si="7">F18+E18</f>
@@ -1019,15 +1029,15 @@
       </c>
       <c r="E19">
         <f>B19/$I$4</f>
-        <v>6.875</v>
+        <v>6.8683034041809234</v>
       </c>
       <c r="F19">
         <f>G20</f>
-        <v>16.125</v>
+        <v>15.931696595819076</v>
       </c>
       <c r="G19">
         <f t="shared" si="7"/>
-        <v>23</v>
+        <v>22.8</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1048,7 +1058,7 @@
       </c>
       <c r="E20">
         <f>$I$3-E19-E18</f>
-        <v>3.625</v>
+        <v>3.4316965958190764</v>
       </c>
       <c r="F20">
         <f>$G$3</f>
@@ -1056,7 +1066,7 @@
       </c>
       <c r="G20">
         <f t="shared" si="7"/>
-        <v>16.125</v>
+        <v>15.931696595819076</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1076,11 +1086,12 @@
         <v>23.5</v>
       </c>
       <c r="E21">
-        <v>0.5</v>
+        <f>E11</f>
+        <v>0.7</v>
       </c>
       <c r="F21">
         <f>G22</f>
-        <v>11</v>
+        <v>10.8</v>
       </c>
       <c r="G21">
         <f t="shared" si="7"/>
@@ -1105,15 +1116,15 @@
       </c>
       <c r="E22">
         <f>B22/$I$4</f>
-        <v>6.875</v>
+        <v>6.8683034041809234</v>
       </c>
       <c r="F22">
         <f>G23</f>
-        <v>4.125</v>
+        <v>3.9316965958190764</v>
       </c>
       <c r="G22">
         <f t="shared" si="7"/>
-        <v>11</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1134,7 +1145,7 @@
       </c>
       <c r="E23">
         <f>$I$3-E22-E21</f>
-        <v>3.625</v>
+        <v>3.4316965958190764</v>
       </c>
       <c r="F23">
         <f>$G$4</f>
@@ -1142,7 +1153,7 @@
       </c>
       <c r="G23">
         <f t="shared" si="7"/>
-        <v>4.125</v>
+        <v>3.9316965958190764</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1167,11 +1178,12 @@
         <v>35.5</v>
       </c>
       <c r="E25">
-        <v>0.5</v>
+        <f>E11</f>
+        <v>0.7</v>
       </c>
       <c r="F25">
         <f>G26</f>
-        <v>23</v>
+        <v>22.8</v>
       </c>
       <c r="G25">
         <f t="shared" ref="G25:G30" si="11">F25+E25</f>
@@ -1196,15 +1208,15 @@
       </c>
       <c r="E26">
         <f>B26/$I$4</f>
-        <v>6.875</v>
+        <v>6.8683034041809234</v>
       </c>
       <c r="F26">
         <f>G27</f>
-        <v>16.125</v>
+        <v>15.931696595819076</v>
       </c>
       <c r="G26">
         <f t="shared" si="11"/>
-        <v>23</v>
+        <v>22.8</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1225,7 +1237,7 @@
       </c>
       <c r="E27">
         <f>$I$3-E26-E25</f>
-        <v>3.625</v>
+        <v>3.4316965958190764</v>
       </c>
       <c r="F27">
         <f>$G$3</f>
@@ -1233,7 +1245,7 @@
       </c>
       <c r="G27">
         <f t="shared" si="11"/>
-        <v>16.125</v>
+        <v>15.931696595819076</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1253,11 +1265,12 @@
         <v>35.5</v>
       </c>
       <c r="E28">
-        <v>0.5</v>
+        <f>E11</f>
+        <v>0.7</v>
       </c>
       <c r="F28">
         <f>G29</f>
-        <v>11</v>
+        <v>10.8</v>
       </c>
       <c r="G28">
         <f t="shared" si="11"/>
@@ -1282,15 +1295,15 @@
       </c>
       <c r="E29">
         <f>B29/$I$4</f>
-        <v>6.875</v>
+        <v>6.8683034041809234</v>
       </c>
       <c r="F29">
         <f>G30</f>
-        <v>4.125</v>
+        <v>3.9316965958190764</v>
       </c>
       <c r="G29">
         <f t="shared" si="11"/>
-        <v>11</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1311,7 +1324,7 @@
       </c>
       <c r="E30">
         <f>$I$3-E29-E28</f>
-        <v>3.625</v>
+        <v>3.4316965958190764</v>
       </c>
       <c r="F30">
         <f>$G$4</f>
@@ -1319,7 +1332,7 @@
       </c>
       <c r="G30">
         <f t="shared" si="11"/>
-        <v>4.125</v>
+        <v>3.9316965958190764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>